<commit_message>
Correcting the Phase 2 probabilities so that they sum to 1 on the last week of gestation.
</commit_message>
<xml_diff>
--- a/Scenario 10.xlsx
+++ b/Scenario 10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/Multiple_outcomes_pregnancy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79419E2B-0B64-B443-955C-CFC0A646E1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5650F120-A919-6443-A317-11EADBA45295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase1" sheetId="6" r:id="rId1"/>
@@ -485,9 +485,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -525,7 +525,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -631,7 +631,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -773,7 +773,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -892,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
@@ -1670,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E296094E-C959-F34D-935C-7330539695AA}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2484,8 +2484,8 @@
         <v>8.6400000000000008E-4</v>
       </c>
       <c r="D42">
-        <f>1*Phase1!C42</f>
-        <v>0.99892000000000003</v>
+        <f>1-C42</f>
+        <v>0.99913600000000002</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -5204,15 +5204,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -5437,15 +5428,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5462,4 +5454,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>